<commit_message>
Updated ALS - Requirements Traceability Matrix - SRD
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
+++ b/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer2\Documents\Not Mine - KIMMY\QUALITY\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV_IT111_GRP_5\apc-softdev-it111-05\documentation\quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
   <si>
     <t>Project Name:</t>
   </si>
@@ -83,21 +83,6 @@
     <t>Joshua C. Dimapilis</t>
   </si>
   <si>
-    <t>001</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>003</t>
-  </si>
-  <si>
-    <t>004</t>
-  </si>
-  <si>
-    <t>005</t>
-  </si>
-  <si>
     <t>Project Adviser/s:</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
   </si>
   <si>
     <t>Ms. Ma. Theresa Montemayor (Database Design and Management)</t>
-  </si>
-  <si>
-    <t>006</t>
   </si>
   <si>
     <t>A. SYSTEM REQUIREMENTS</t>
@@ -186,22 +168,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unregistered users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to sign up for membership</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Allows </t>
+      <t>registered users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
     </r>
     <r>
       <rPr>
@@ -213,17 +190,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>registered users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
+      <t>admin or member roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) to listen to audio files included in the calendar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allows </t>
     </r>
     <r>
       <rPr>
@@ -235,22 +217,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>admin or member roles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) to listen to audio files included in the calendar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Allows </t>
+      <t xml:space="preserve">users with admin role </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to add calendar events</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Does not allow </t>
     </r>
     <r>
       <rPr>
@@ -262,17 +244,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">users with admin role </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to add calendar events</t>
+      <t>unregistered users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to view the calendar and calendar events</t>
     </r>
   </si>
   <si>
@@ -289,22 +271,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">users with admin roles </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to delete calendar events</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Does not allow </t>
+      <t>registered users</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
     </r>
     <r>
       <rPr>
@@ -316,22 +293,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>unregistered users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> to view the calendar and calendar events</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Allows </t>
+      <t>admin or member roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>) to view the calendar and calendar events</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
     </r>
     <r>
       <rPr>
@@ -343,22 +320,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users with admin roles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>to update or modify calendar events</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Allows </t>
+      <t>users with admin role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, he/she can perform </t>
     </r>
     <r>
       <rPr>
@@ -370,17 +342,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>registered users</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (</t>
+      <t>create</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function in the calendar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
     </r>
     <r>
       <rPr>
@@ -392,40 +369,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>admin or member roles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>) to view the calendar and calendar events</t>
-    </r>
-  </si>
-  <si>
-    <t>007</t>
-  </si>
-  <si>
-    <t>008</t>
-  </si>
-  <si>
-    <t>009</t>
-  </si>
-  <si>
-    <t>User must have a username and a password to access the website</t>
-  </si>
-  <si>
-    <t>User must access the website using the login page</t>
-  </si>
-  <si>
-    <t>User can view the calendar</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
+      <t>users with admin role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, he/she can perform </t>
     </r>
     <r>
       <rPr>
@@ -437,17 +391,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users with admin role</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, he/she can perform </t>
+      <t>update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function in the calendar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
     </r>
     <r>
       <rPr>
@@ -459,22 +418,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>create</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> function in the calendar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
+      <t>users with admin role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, he/she can perform </t>
     </r>
     <r>
       <rPr>
@@ -486,17 +440,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users with admin role</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, he/she can perform </t>
+      <t>delete</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> function in the calendar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">For </t>
     </r>
     <r>
       <rPr>
@@ -508,22 +467,17 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>update</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> function in the calendar</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
+      <t>users with admin/member role</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, he/she can </t>
     </r>
     <r>
       <rPr>
@@ -535,17 +489,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users with admin role</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, he/she can perform </t>
+      <t>read</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the contents of the calendar</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Filters the calendar if specific year is chosen by the user (</t>
     </r>
     <r>
       <rPr>
@@ -557,28 +516,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>delete</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> function in the calendar</t>
-    </r>
-  </si>
-  <si>
-    <t>User can listen to audio files provided in the calendar</t>
-  </si>
-  <si>
-    <t>User can click links</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">User can view the calendar in a </t>
+      <t>admin or member roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Filters the calendar if specific month is chosen by the user (</t>
     </r>
     <r>
       <rPr>
@@ -590,15 +543,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>monthly basis</t>
-    </r>
-  </si>
-  <si>
-    <t>User can navigate through the different months of the year</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">For </t>
+      <t>admin or member roles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updates the calendar display if </t>
     </r>
     <r>
       <rPr>
@@ -610,17 +570,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>users with admin/member role</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, he/she can </t>
+      <t xml:space="preserve">CRUD function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>is performed by the user</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Updates the system database if </t>
     </r>
     <r>
       <rPr>
@@ -632,79 +597,40 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>read</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> the contents of the calendar</t>
-    </r>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
-    <t>011</t>
-  </si>
-  <si>
-    <t>012</t>
-  </si>
-  <si>
-    <t>013</t>
-  </si>
-  <si>
-    <t>014</t>
-  </si>
-  <si>
-    <t>015</t>
-  </si>
-  <si>
-    <t>016</t>
-  </si>
-  <si>
-    <t>017</t>
-  </si>
-  <si>
-    <t>018</t>
-  </si>
-  <si>
-    <t>019</t>
-  </si>
-  <si>
-    <t>020</t>
-  </si>
-  <si>
-    <t>021</t>
-  </si>
-  <si>
-    <t>User can click buttons or tabs within the page</t>
-  </si>
-  <si>
-    <t>User can choose a specific year to navigate</t>
-  </si>
-  <si>
-    <t>User can choose a specific month to navigate</t>
-  </si>
-  <si>
-    <t>User can view Sunday Readings</t>
-  </si>
-  <si>
-    <t>User can view Weekday Readings</t>
-  </si>
-  <si>
-    <t>User can click audio files provided in the calendar</t>
-  </si>
-  <si>
-    <t>User can play the audio files provided in the calendar</t>
-  </si>
-  <si>
-    <r>
-      <t>Filters the calendar if specific year is chosen by the user (</t>
+      <t xml:space="preserve">CRUD function </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">is performed by the user </t>
+    </r>
+  </si>
+  <si>
+    <t>System Interface</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>HIgh</t>
+  </si>
+  <si>
+    <t>Registered user can click buttons or tabs within the page</t>
+  </si>
+  <si>
+    <t>Registered user can play the audio files provided in the calendar</t>
+  </si>
+  <si>
+    <t>Registered user can listen to audio files provided in the calendar</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Registered user can view the calendar in a </t>
     </r>
     <r>
       <rPr>
@@ -716,22 +642,30 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>admin or member roles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Filters the calendar if specific month is chosen by the user (</t>
+      <t>monthly basis</t>
+    </r>
+  </si>
+  <si>
+    <t>Registered user can choose a specific year to navigate</t>
+  </si>
+  <si>
+    <t>Registered user can choose a specific month to navigate</t>
+  </si>
+  <si>
+    <t>Registered user can view Weekday Readings</t>
+  </si>
+  <si>
+    <t>Registered user can view Sunday Readings</t>
+  </si>
+  <si>
+    <t>Provides a sign up page to allow unregistered users to register and access the site</t>
+  </si>
+  <si>
+    <t>Provides a user-friendly interface for easier navigation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allows </t>
     </r>
     <r>
       <rPr>
@@ -743,22 +677,22 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>admin or member roles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Updates the calendar display if </t>
+      <t xml:space="preserve">users with admin role </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to delete calendar events</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allows </t>
     </r>
     <r>
       <rPr>
@@ -770,48 +704,96 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">CRUD function </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>is performed by the user</t>
-    </r>
-  </si>
-  <si>
-    <t>Database</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Updates the system database if </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">CRUD function </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">is performed by the user </t>
-    </r>
+      <t xml:space="preserve">users with admin role </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>to update or modify calendar events</t>
+    </r>
+  </si>
+  <si>
+    <t>Registered user can click audio files provided in the calendar</t>
+  </si>
+  <si>
+    <t>Registered user can click links</t>
+  </si>
+  <si>
+    <t>Registered user must have a username and a password to access the website</t>
+  </si>
+  <si>
+    <t>Registered user must access the website using the login page</t>
+  </si>
+  <si>
+    <t>Registered user can navigate through the different months/years of the calendar</t>
+  </si>
+  <si>
+    <t>001</t>
+  </si>
+  <si>
+    <t>002</t>
+  </si>
+  <si>
+    <t>003</t>
+  </si>
+  <si>
+    <t>004</t>
+  </si>
+  <si>
+    <t>005</t>
+  </si>
+  <si>
+    <t>006</t>
+  </si>
+  <si>
+    <t>007</t>
+  </si>
+  <si>
+    <t>008</t>
+  </si>
+  <si>
+    <t>009</t>
+  </si>
+  <si>
+    <t>010</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
   </si>
   <si>
     <t>022</t>
@@ -848,7 +830,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -893,6 +875,12 @@
       <i/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1006,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1053,6 +1041,12 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1079,9 +1073,6 @@
     </xf>
     <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1365,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:J8"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,168 +1376,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="26">
         <v>42016</v>
       </c>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="26">
         <v>42106</v>
       </c>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
+        <v>19</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
+      <c r="B7" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
+      <c r="B8" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
+      <c r="B9" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="19"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
-      <c r="J11" s="20"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="22"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="22"/>
+      <c r="E11" s="22"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="22"/>
+      <c r="H11" s="22"/>
+      <c r="I11" s="22"/>
+      <c r="J11" s="22"/>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1581,37 +1572,37 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13" s="21"/>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="22"/>
+      <c r="A13" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>19</v>
+        <v>67</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>33</v>
+        <v>59</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="14" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
@@ -1620,22 +1611,22 @@
     </row>
     <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G15" s="14"/>
       <c r="H15" s="14"/>
@@ -1644,22 +1635,22 @@
     </row>
     <row r="16" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>21</v>
+        <v>69</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E16" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="14"/>
@@ -1668,22 +1659,22 @@
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>33</v>
+        <v>30</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="G17" s="14"/>
       <c r="H17" s="14"/>
@@ -1692,22 +1683,22 @@
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E18" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G18" s="14"/>
       <c r="H18" s="14"/>
@@ -1716,22 +1707,22 @@
     </row>
     <row r="19" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="B19" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="F19" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="G19" s="14"/>
       <c r="H19" s="14"/>
@@ -1740,20 +1731,22 @@
     </row>
     <row r="20" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="B20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="10" t="s">
+      <c r="C20" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
@@ -1762,42 +1755,46 @@
     </row>
     <row r="21" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D21" s="14"/>
-      <c r="E21" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E21" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G21" s="14"/>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
     </row>
-    <row r="22" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="14"/>
-      <c r="E22" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
@@ -1806,22 +1803,20 @@
     </row>
     <row r="23" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="E23" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F23" s="14" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -1830,22 +1825,20 @@
     </row>
     <row r="24" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E24" s="15" t="s">
-        <v>37</v>
+        <v>61</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="14"/>
+      <c r="E24" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F24" s="14" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
@@ -1854,20 +1847,20 @@
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="12" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="F25" s="14" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
@@ -1876,40 +1869,51 @@
     </row>
     <row r="26" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>38</v>
+        <v>45</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D26" s="14"/>
-      <c r="E26" s="15" t="s">
-        <v>37</v>
+      <c r="E26" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F26" s="14" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="14"/>
+    <row r="27" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="E27" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>29</v>
+      </c>
       <c r="G27" s="14"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
     </row>
-    <row r="28" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
+      <c r="B28" s="13"/>
       <c r="C28" s="14"/>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -1919,86 +1923,73 @@
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="17"/>
-      <c r="J29" s="18"/>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B30" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30" s="10" t="s">
+    <row r="29" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="12"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D30" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="10" t="s">
-        <v>33</v>
+        <v>64</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>32</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>31</v>
+        <v>26</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="F31" s="14" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G31" s="14"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F32" s="14" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -2007,20 +1998,22 @@
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D33" s="14"/>
-      <c r="E33" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E33" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F33" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G33" s="14"/>
       <c r="H33" s="14"/>
@@ -2029,22 +2022,22 @@
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F34" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -2053,20 +2046,22 @@
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="14"/>
-      <c r="E35" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E35" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F35" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G35" s="14"/>
       <c r="H35" s="14"/>
@@ -2075,44 +2070,46 @@
     </row>
     <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D36" s="14"/>
-      <c r="E36" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F36" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G36" s="14"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="C37" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E37" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F37" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G37" s="14"/>
       <c r="H37" s="14"/>
@@ -2121,22 +2118,22 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C38" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E38" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F38" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G38" s="14"/>
       <c r="H38" s="14"/>
@@ -2145,22 +2142,20 @@
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B39" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="C39" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="14"/>
+      <c r="E39" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F39" s="14" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
@@ -2169,22 +2164,22 @@
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>80</v>
+        <v>42</v>
       </c>
       <c r="C40" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E40" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F40" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G40" s="14"/>
       <c r="H40" s="14"/>
@@ -2193,22 +2188,20 @@
     </row>
     <row r="41" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="12" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B41" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E41" s="15" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="14"/>
+      <c r="E41" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F41" s="14" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
@@ -2217,22 +2210,20 @@
     </row>
     <row r="42" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="12" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B42" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E42" s="15" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="14"/>
+      <c r="E42" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="F42" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
@@ -2241,22 +2232,22 @@
     </row>
     <row r="43" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="12" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B43" s="13" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C43" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E43" s="15" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G43" s="14"/>
       <c r="H43" s="14"/>
@@ -2265,94 +2256,94 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="12" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B44" s="13" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E44" s="25" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E44" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="F44" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="12" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B45" s="13" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="C45" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E45" s="25" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="F45" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="12" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B46" s="13" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C46" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="F46" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B47" s="13" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="C47" s="15" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E47" s="25" t="s">
-        <v>37</v>
+        <v>26</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>31</v>
       </c>
       <c r="F47" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="G47" s="14"/>
       <c r="H47" s="14"/>
@@ -2379,7 +2370,7 @@
     <mergeCell ref="B3:J3"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B4:J4"/>
-    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="A11:J11"/>
     <mergeCell ref="B7:J7"/>

</xml_diff>

<commit_message>
Updated ALS - Requirements Traceability Matrix - SRD.xlsx
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
+++ b/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV_IT111_GRP_5\apc-softdev-it111-05\documentation\quality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV_IT111(GRP 5)\apc-softdev-it111-05\documentation\quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
   <si>
     <t>Project Name:</t>
   </si>
@@ -824,6 +824,28 @@
   </si>
   <si>
     <t>031</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>3.2.1
+3.3.3</t>
+  </si>
+  <si>
+    <t>3.3.4</t>
+  </si>
+  <si>
+    <t>3.3.4.1</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1047,6 +1069,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1056,9 +1090,6 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1068,11 +1099,11 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1399,7 @@
     <col min="4" max="4" width="12.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="9" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="29" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="9" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" style="9" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="9" customWidth="1"/>
@@ -1376,168 +1407,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="21">
         <v>42016</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="21">
         <v>42106</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1558,7 +1589,7 @@
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -1572,18 +1603,18 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -1604,7 +1635,7 @@
       <c r="F14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1628,7 +1659,9 @@
       <c r="F15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1652,7 +1685,9 @@
       <c r="F16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="28" t="s">
+        <v>98</v>
+      </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -1676,7 +1711,9 @@
       <c r="F17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="28" t="s">
+        <v>99</v>
+      </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -1700,7 +1737,9 @@
       <c r="F18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1724,7 +1763,7 @@
       <c r="F19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1748,7 +1787,9 @@
       <c r="F20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="14"/>
+      <c r="G20" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1772,7 +1813,9 @@
       <c r="F21" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="14"/>
+      <c r="G21" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -1796,7 +1839,7 @@
       <c r="F22" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -1818,7 +1861,7 @@
       <c r="F23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1840,7 +1883,7 @@
       <c r="F24" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="14"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1862,7 +1905,7 @@
       <c r="F25" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -1884,7 +1927,7 @@
       <c r="F26" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -1906,7 +1949,7 @@
       <c r="F27" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -1918,7 +1961,7 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -1929,24 +1972,24 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
@@ -1967,7 +2010,7 @@
       <c r="F31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -1991,7 +2034,9 @@
       <c r="F32" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -2015,7 +2060,9 @@
       <c r="F33" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="28" t="s">
+        <v>99</v>
+      </c>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -2039,7 +2086,9 @@
       <c r="F34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="14"/>
+      <c r="G34" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -2063,7 +2112,7 @@
       <c r="F35" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="14"/>
+      <c r="G35" s="28"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -2087,7 +2136,7 @@
       <c r="F36" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="14"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -2111,7 +2160,7 @@
       <c r="F37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="14"/>
+      <c r="G37" s="28"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -2135,7 +2184,7 @@
       <c r="F38" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="28"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -2157,7 +2206,7 @@
       <c r="F39" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -2181,7 +2230,9 @@
       <c r="F40" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="14"/>
+      <c r="G40" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -2203,7 +2254,7 @@
       <c r="F41" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="14"/>
+      <c r="G41" s="28"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -2225,7 +2276,7 @@
       <c r="F42" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="14"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -2249,7 +2300,7 @@
       <c r="F43" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="14"/>
+      <c r="G43" s="28"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -2273,7 +2324,7 @@
       <c r="F44" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="14"/>
+      <c r="G44" s="28"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -2297,7 +2348,7 @@
       <c r="F45" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="14"/>
+      <c r="G45" s="28"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -2321,7 +2372,7 @@
       <c r="F46" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G46" s="14"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -2345,7 +2396,7 @@
       <c r="F47" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G47" s="14"/>
+      <c r="G47" s="28"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -2357,19 +2408,13 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
+      <c r="G48" s="28"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B4:J4"/>
     <mergeCell ref="A30:J30"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="A11:J11"/>
@@ -2377,6 +2422,12 @@
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A13:J13"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modified files for quality
</commit_message>
<xml_diff>
--- a/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
+++ b/documentation/quality/ALS - Requirements Traceability Matrix - SRD.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV_IT111_GRP_5\apc-softdev-it111-05\documentation\quality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SOFTDEV_IT111(GRP 5)\apc-softdev-it111-05\documentation\quality\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="105">
   <si>
     <t>Project Name:</t>
   </si>
@@ -824,6 +824,28 @@
   </si>
   <si>
     <t>031</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>3.2.1</t>
+  </si>
+  <si>
+    <t>3.1.3</t>
+  </si>
+  <si>
+    <t>3.2.1
+3.3.3</t>
+  </si>
+  <si>
+    <t>3.3.4</t>
+  </si>
+  <si>
+    <t>3.3.4.1</t>
+  </si>
+  <si>
+    <t>3.3.2</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1016,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1047,6 +1069,18 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1056,9 +1090,6 @@
     <xf numFmtId="49" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1068,11 +1099,11 @@
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1356,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1399,7 @@
     <col min="4" max="4" width="12.42578125" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="9" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="9" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="29" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" style="9" customWidth="1"/>
     <col min="9" max="9" width="13.85546875" style="9" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="9" customWidth="1"/>
@@ -1376,168 +1407,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="21">
         <v>42016</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+      <c r="I4" s="19"/>
+      <c r="J4" s="19"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="21">
         <v>42106</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="22"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="25"/>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
     </row>
     <row r="12" spans="1:10" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
@@ -1558,7 +1589,7 @@
       <c r="F12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="18" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="6" t="s">
@@ -1572,18 +1603,18 @@
       </c>
     </row>
     <row r="13" spans="1:10" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="J13" s="27"/>
     </row>
     <row r="14" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
@@ -1604,7 +1635,7 @@
       <c r="F14" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="14"/>
+      <c r="G14" s="28"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
       <c r="J14" s="14"/>
@@ -1628,7 +1659,9 @@
       <c r="F15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G15" s="14"/>
+      <c r="G15" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="H15" s="14"/>
       <c r="I15" s="14"/>
       <c r="J15" s="14"/>
@@ -1652,7 +1685,9 @@
       <c r="F16" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="14"/>
+      <c r="G16" s="28" t="s">
+        <v>98</v>
+      </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="14"/>
@@ -1676,7 +1711,9 @@
       <c r="F17" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="28" t="s">
+        <v>99</v>
+      </c>
       <c r="H17" s="14"/>
       <c r="I17" s="14"/>
       <c r="J17" s="14"/>
@@ -1700,7 +1737,9 @@
       <c r="F18" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G18" s="14"/>
+      <c r="G18" s="28" t="s">
+        <v>101</v>
+      </c>
       <c r="H18" s="14"/>
       <c r="I18" s="14"/>
       <c r="J18" s="14"/>
@@ -1724,7 +1763,7 @@
       <c r="F19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="28"/>
       <c r="H19" s="14"/>
       <c r="I19" s="14"/>
       <c r="J19" s="14"/>
@@ -1748,7 +1787,9 @@
       <c r="F20" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G20" s="14"/>
+      <c r="G20" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="H20" s="14"/>
       <c r="I20" s="14"/>
       <c r="J20" s="14"/>
@@ -1772,7 +1813,9 @@
       <c r="F21" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G21" s="14"/>
+      <c r="G21" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
@@ -1796,7 +1839,7 @@
       <c r="F22" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="14"/>
+      <c r="G22" s="28"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
@@ -1818,7 +1861,7 @@
       <c r="F23" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="28"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
@@ -1840,7 +1883,7 @@
       <c r="F24" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="14"/>
+      <c r="G24" s="28"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
@@ -1862,7 +1905,7 @@
       <c r="F25" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G25" s="14"/>
+      <c r="G25" s="28"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
@@ -1884,7 +1927,7 @@
       <c r="F26" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G26" s="14"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
@@ -1906,7 +1949,7 @@
       <c r="F27" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="28"/>
       <c r="H27" s="14"/>
       <c r="I27" s="14"/>
       <c r="J27" s="14"/>
@@ -1918,7 +1961,7 @@
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
+      <c r="G28" s="28"/>
       <c r="H28" s="14"/>
       <c r="I28" s="14"/>
       <c r="J28" s="14"/>
@@ -1929,24 +1972,24 @@
       <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
+      <c r="G29" s="28"/>
       <c r="H29" s="14"/>
       <c r="I29" s="14"/>
       <c r="J29" s="14"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="19"/>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="20"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
@@ -1967,7 +2010,7 @@
       <c r="F31" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G31" s="14"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
@@ -1991,7 +2034,9 @@
       <c r="F32" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="G32" s="14"/>
+      <c r="G32" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="H32" s="14"/>
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
@@ -2015,7 +2060,9 @@
       <c r="F33" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G33" s="14"/>
+      <c r="G33" s="28" t="s">
+        <v>99</v>
+      </c>
       <c r="H33" s="14"/>
       <c r="I33" s="14"/>
       <c r="J33" s="14"/>
@@ -2039,7 +2086,9 @@
       <c r="F34" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="14"/>
+      <c r="G34" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="H34" s="14"/>
       <c r="I34" s="14"/>
       <c r="J34" s="14"/>
@@ -2063,7 +2112,7 @@
       <c r="F35" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G35" s="14"/>
+      <c r="G35" s="28"/>
       <c r="H35" s="14"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
@@ -2087,7 +2136,7 @@
       <c r="F36" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G36" s="14"/>
+      <c r="G36" s="28"/>
       <c r="H36" s="14"/>
       <c r="I36" s="14"/>
       <c r="J36" s="14"/>
@@ -2111,7 +2160,7 @@
       <c r="F37" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="14"/>
+      <c r="G37" s="28"/>
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
@@ -2135,7 +2184,7 @@
       <c r="F38" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G38" s="14"/>
+      <c r="G38" s="28"/>
       <c r="H38" s="14"/>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -2157,7 +2206,7 @@
       <c r="F39" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G39" s="14"/>
+      <c r="G39" s="28"/>
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
@@ -2181,7 +2230,9 @@
       <c r="F40" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="14"/>
+      <c r="G40" s="28" t="s">
+        <v>104</v>
+      </c>
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
@@ -2203,7 +2254,7 @@
       <c r="F41" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="14"/>
+      <c r="G41" s="28"/>
       <c r="H41" s="14"/>
       <c r="I41" s="14"/>
       <c r="J41" s="14"/>
@@ -2225,7 +2276,7 @@
       <c r="F42" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G42" s="14"/>
+      <c r="G42" s="28"/>
       <c r="H42" s="14"/>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -2249,7 +2300,7 @@
       <c r="F43" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G43" s="14"/>
+      <c r="G43" s="28"/>
       <c r="H43" s="14"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14"/>
@@ -2273,7 +2324,7 @@
       <c r="F44" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="14"/>
+      <c r="G44" s="28"/>
       <c r="H44" s="14"/>
       <c r="I44" s="14"/>
       <c r="J44" s="14"/>
@@ -2297,7 +2348,7 @@
       <c r="F45" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G45" s="14"/>
+      <c r="G45" s="28"/>
       <c r="H45" s="14"/>
       <c r="I45" s="14"/>
       <c r="J45" s="14"/>
@@ -2321,7 +2372,7 @@
       <c r="F46" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G46" s="14"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="14"/>
       <c r="I46" s="14"/>
       <c r="J46" s="14"/>
@@ -2345,7 +2396,7 @@
       <c r="F47" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G47" s="14"/>
+      <c r="G47" s="28"/>
       <c r="H47" s="14"/>
       <c r="I47" s="14"/>
       <c r="J47" s="14"/>
@@ -2357,19 +2408,13 @@
       <c r="D48" s="14"/>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
+      <c r="G48" s="28"/>
       <c r="H48" s="14"/>
       <c r="I48" s="14"/>
       <c r="J48" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B6:J6"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B5:J5"/>
-    <mergeCell ref="B4:J4"/>
     <mergeCell ref="A30:J30"/>
     <mergeCell ref="B10:J10"/>
     <mergeCell ref="A11:J11"/>
@@ -2377,6 +2422,12 @@
     <mergeCell ref="B8:J8"/>
     <mergeCell ref="B9:J9"/>
     <mergeCell ref="A13:J13"/>
+    <mergeCell ref="B6:J6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="B5:J5"/>
+    <mergeCell ref="B4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>